<commit_message>
Oracle ODP.NET (managed) added. MsSql JDBC added.
Not included in result (for now).
</commit_message>
<xml_diff>
--- a/GatherResults/template.xlsx
+++ b/GatherResults/template.xlsx
@@ -14,13 +14,13 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="30" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="90">
   <si>
     <t>Simple</t>
   </si>
@@ -127,9 +127,6 @@
     <t>[[bench.complexRelations.searchAll]]</t>
   </si>
   <si>
-    <t>Search subset (x5.000)</t>
-  </si>
-  <si>
     <t>[[bench.simple.searchSubset]]</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>[[bench.complexRelations.queryFilter]]</t>
   </si>
   <si>
-    <t>Find many (x10.000)</t>
-  </si>
-  <si>
     <t>[[bench.simple.findMany]]</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
     <t>[[bench.complexRelations.findMany]]</t>
   </si>
   <si>
-    <t>Find one (x10.000)</t>
-  </si>
-  <si>
     <t>[[bench.simple.findOne]]</t>
   </si>
   <si>
@@ -272,6 +263,33 @@
   </si>
   <si>
     <t>Find one (x5.000)</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>[[database]]</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>[[platform]]</t>
+  </si>
+  <si>
+    <t>ORM</t>
+  </si>
+  <si>
+    <t>[[orm]]</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>[[api]]</t>
+  </si>
+  <si>
+    <t>(All)</t>
   </si>
 </sst>
 </file>
@@ -363,7 +381,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -452,7 +469,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Simple!$B$1:$B$2</c:f>
+              <c:f>Simple!$B$6:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -464,7 +481,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Simple!$A$3:$A$14</c:f>
+              <c:f>Simple!$A$8:$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -474,38 +491,38 @@
                   <c:v>Bulk update</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Find many (x10.000)</c:v>
+                  <c:v>Loop insert (half)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Find one (x10.000)</c:v>
+                  <c:v>Loop update (half)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Loop insert (half)</c:v>
+                  <c:v>Query all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Loop update (half)</c:v>
+                  <c:v>Report (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Query all (x100)</c:v>
+                  <c:v>Search all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Report (x1.000)</c:v>
+                  <c:v>Query filter (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Search all (x100)</c:v>
+                  <c:v>Search subset (x3.000)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Search subset (x5.000)</c:v>
+                  <c:v>Find many (x2.000)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Query filter (x1.000)</c:v>
+                  <c:v>Find one (x5.000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Simple!$B$3:$B$14</c:f>
+              <c:f>Simple!$B$8:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -555,11 +572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="219424256"/>
-        <c:axId val="219425792"/>
+        <c:axId val="142661504"/>
+        <c:axId val="161653888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219424256"/>
+        <c:axId val="142661504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,7 +585,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219425792"/>
+        <c:crossAx val="161653888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,48 +593,26 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219425792"/>
+        <c:axId val="161653888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>ms</a:t>
-                </a:r>
-                <a:endParaRPr lang="hr-HR"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219424256"/>
+        <c:crossAx val="142661504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-      </c:dTable>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -633,6 +628,7 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -679,7 +675,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -906,7 +901,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Standard!$B$1:$B$3</c:f>
+              <c:f>Standard!$B$6:$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -918,7 +913,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Standard!$A$4:$A$15</c:f>
+              <c:f>Standard!$A$9:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -928,38 +923,38 @@
                   <c:v>Bulk update</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Find many (x10.000)</c:v>
+                  <c:v>Loop insert (half)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Find one (x10.000)</c:v>
+                  <c:v>Loop update (half)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Loop insert (half)</c:v>
+                  <c:v>Query all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Loop update (half)</c:v>
+                  <c:v>Report (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Query all (x100)</c:v>
+                  <c:v>Search all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Report (x1.000)</c:v>
+                  <c:v>Query filter (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Search all (x100)</c:v>
+                  <c:v>Search subset (x3.000)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Search subset (x5.000)</c:v>
+                  <c:v>Find many (x2.000)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Query filter (x1.000)</c:v>
+                  <c:v>Find one (x5.000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Standard!$B$4:$B$15</c:f>
+              <c:f>Standard!$B$9:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1005,7 +1000,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Standard!$C$1:$C$3</c:f>
+              <c:f>Standard!$C$6:$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1017,7 +1012,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Standard!$A$4:$A$15</c:f>
+              <c:f>Standard!$A$9:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1027,38 +1022,38 @@
                   <c:v>Bulk update</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Find many (x10.000)</c:v>
+                  <c:v>Loop insert (half)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Find one (x10.000)</c:v>
+                  <c:v>Loop update (half)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Loop insert (half)</c:v>
+                  <c:v>Query all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Loop update (half)</c:v>
+                  <c:v>Report (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Query all (x100)</c:v>
+                  <c:v>Search all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Report (x1.000)</c:v>
+                  <c:v>Query filter (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Search all (x100)</c:v>
+                  <c:v>Search subset (x3.000)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Search subset (x5.000)</c:v>
+                  <c:v>Find many (x2.000)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Query filter (x1.000)</c:v>
+                  <c:v>Find one (x5.000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Standard!$C$4:$C$15</c:f>
+              <c:f>Standard!$C$9:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1108,11 +1103,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="219826432"/>
-        <c:axId val="219848704"/>
+        <c:axId val="192604800"/>
+        <c:axId val="192869504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219826432"/>
+        <c:axId val="192604800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,7 +1116,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219848704"/>
+        <c:crossAx val="192869504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1129,48 +1124,26 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219848704"/>
+        <c:axId val="192869504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>ms</a:t>
-                </a:r>
-                <a:endParaRPr lang="hr-HR"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219826432"/>
+        <c:crossAx val="192604800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-      </c:dTable>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1186,6 +1159,7 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -1232,7 +1206,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1591,7 +1564,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Complex!$B$1:$B$3</c:f>
+              <c:f>Complex!$B$6:$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1603,7 +1576,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Complex!$A$4:$A$15</c:f>
+              <c:f>Complex!$A$9:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1613,38 +1586,38 @@
                   <c:v>Bulk update</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Find many (x10.000)</c:v>
+                  <c:v>Loop insert (half)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Find one (x10.000)</c:v>
+                  <c:v>Loop update (half)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Loop insert (half)</c:v>
+                  <c:v>Query all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Loop update (half)</c:v>
+                  <c:v>Report (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Query all (x100)</c:v>
+                  <c:v>Search all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Report (x1.000)</c:v>
+                  <c:v>Query filter (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Search all (x100)</c:v>
+                  <c:v>Search subset (x3.000)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Search subset (x5.000)</c:v>
+                  <c:v>Find many (x2.000)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Query filter (x1.000)</c:v>
+                  <c:v>Find one (x5.000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Complex!$B$4:$B$15</c:f>
+              <c:f>Complex!$B$9:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1690,7 +1663,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Complex!$C$1:$C$3</c:f>
+              <c:f>Complex!$C$6:$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1702,7 +1675,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Complex!$A$4:$A$15</c:f>
+              <c:f>Complex!$A$9:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1712,38 +1685,38 @@
                   <c:v>Bulk update</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Find many (x10.000)</c:v>
+                  <c:v>Loop insert (half)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Find one (x10.000)</c:v>
+                  <c:v>Loop update (half)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Loop insert (half)</c:v>
+                  <c:v>Query all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Loop update (half)</c:v>
+                  <c:v>Report (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Query all (x100)</c:v>
+                  <c:v>Search all (x100)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Report (x1.000)</c:v>
+                  <c:v>Query filter (x1.000)</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Search all (x100)</c:v>
+                  <c:v>Search subset (x3.000)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Search subset (x5.000)</c:v>
+                  <c:v>Find many (x2.000)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Query filter (x1.000)</c:v>
+                  <c:v>Find one (x5.000)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Complex!$C$4:$C$15</c:f>
+              <c:f>Complex!$C$9:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1793,11 +1766,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="220199936"/>
-        <c:axId val="220226304"/>
+        <c:axId val="208032128"/>
+        <c:axId val="208034048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="220199936"/>
+        <c:axId val="208032128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1806,7 +1779,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220226304"/>
+        <c:crossAx val="208034048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1814,48 +1787,26 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220226304"/>
+        <c:axId val="208034048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>ms</a:t>
-                </a:r>
-                <a:endParaRPr lang="hr-HR"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220199936"/>
+        <c:crossAx val="208032128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-      </c:dTable>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1871,6 +1822,7 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -1988,24 +1940,27 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42068.480947453703" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="11">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Rikard Pavelic" refreshedDate="42160.433094907406" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="11">
   <cacheSource type="worksheet">
     <worksheetSource name="Table3"/>
   </cacheSource>
-  <cacheFields count="7">
+  <cacheFields count="11">
     <cacheField name="Bench type" numFmtId="0">
-      <sharedItems count="12">
+      <sharedItems count="15">
         <s v="Bulk insert"/>
         <s v="Bulk update"/>
         <s v="Loop insert (half)"/>
         <s v="Loop update (half)"/>
         <s v="Search all (x100)"/>
-        <s v="Search subset (x5.000)"/>
+        <s v="Search subset (x3.000)"/>
         <s v="Query all (x100)"/>
         <s v="Query filter (x1.000)"/>
-        <s v="Find many (x10.000)"/>
-        <s v="Find one (x10.000)"/>
+        <s v="Find many (x2.000)"/>
+        <s v="Find one (x5.000)"/>
         <s v="Report (x1.000)"/>
+        <s v="Find many (x10.000)" u="1"/>
+        <s v="Search subset (x5.000)" u="1"/>
+        <s v="Find one (x10.000)" u="1"/>
         <s v="Query all (x1.000)" u="1"/>
       </sharedItems>
     </cacheField>
@@ -2029,6 +1984,26 @@
         <s v="[[description]]"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="Database" numFmtId="0">
+      <sharedItems count="1">
+        <s v="[[database]]"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Platform" numFmtId="0">
+      <sharedItems count="1">
+        <s v="[[platform]]"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ORM" numFmtId="0">
+      <sharedItems count="1">
+        <s v="[[orm]]"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="API" numFmtId="0">
+      <sharedItems count="1">
+        <s v="[[api]]"/>
+      </sharedItems>
+    </cacheField>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -2048,6 +2023,10 @@
     <s v="[[bench.complexObjects.bulkInsert]]"/>
     <s v="[[bench.complexRelations.bulkInsert]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
@@ -2057,6 +2036,10 @@
     <s v="[[bench.complexObjects.bulkUpdate]]"/>
     <s v="[[bench.complexRelations.bulkUpdate]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="2"/>
@@ -2066,6 +2049,10 @@
     <s v="[[bench.complexObjects.loopInsertHalf]]"/>
     <s v="[[bench.complexRelations.loopInsertHalf]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="3"/>
@@ -2075,6 +2062,10 @@
     <s v="[[bench.complexObjects.loopUpdateHalf]]"/>
     <s v="[[bench.complexRelations.loopUpdateHalf]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="4"/>
@@ -2084,6 +2075,10 @@
     <s v="[[bench.complexObjects.searchAll]]"/>
     <s v="[[bench.complexRelations.searchAll]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="5"/>
@@ -2093,6 +2088,10 @@
     <s v="[[bench.complexObjects.searchSubset]]"/>
     <s v="[[bench.complexRelations.searchSubset]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="6"/>
@@ -2102,6 +2101,10 @@
     <s v="[[bench.complexObjects.queryAll]]"/>
     <s v="[[bench.complexRelations.queryAll]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="7"/>
@@ -2111,6 +2114,10 @@
     <s v="[[bench.complexObjects.queryFilter]]"/>
     <s v="[[bench.complexRelations.queryFilter]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="8"/>
@@ -2120,6 +2127,10 @@
     <s v="[[bench.complexObjects.findMany]]"/>
     <s v="[[bench.complexRelations.findMany]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="9"/>
@@ -2129,6 +2140,10 @@
     <s v="[[bench.complexObjects.findOne]]"/>
     <s v="[[bench.complexRelations.findOne]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="10"/>
@@ -2138,28 +2153,35 @@
     <s v="[[bench.complexObjects.report]]"/>
     <s v="[[bench.complexRelations.report]]"/>
     <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:C14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A6:C19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
-      <items count="13">
+      <items count="16">
         <item x="0"/>
         <item x="1"/>
-        <item x="8"/>
-        <item x="9"/>
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
         <item x="2"/>
         <item x="3"/>
-        <item m="1" x="11"/>
+        <item m="1" x="14"/>
         <item x="6"/>
         <item x="10"/>
         <item x="4"/>
+        <item m="1" x="12"/>
+        <item x="7"/>
         <item x="5"/>
-        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2174,6 +2196,26 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -2184,12 +2226,6 @@
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i>
       <x v="4"/>
@@ -2207,10 +2243,16 @@
       <x v="9"/>
     </i>
     <i>
-      <x v="10"/>
+      <x v="11"/>
     </i>
     <i>
-      <x v="11"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i t="grand">
       <x/>
@@ -2227,6 +2269,12 @@
       <x/>
     </i>
   </colItems>
+  <pageFields count="4">
+    <pageField fld="10" hier="-1"/>
+    <pageField fld="7" hier="-1"/>
+    <pageField fld="8" hier="-1"/>
+    <pageField fld="9" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Relational" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
@@ -2353,23 +2401,26 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A1:E15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A6:E20" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
-      <items count="13">
+      <items count="16">
         <item x="0"/>
         <item x="1"/>
-        <item x="8"/>
-        <item x="9"/>
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
         <item x="2"/>
         <item x="3"/>
-        <item m="1" x="11"/>
+        <item m="1" x="14"/>
         <item x="6"/>
         <item x="10"/>
         <item x="4"/>
+        <item m="1" x="12"/>
+        <item x="7"/>
         <item x="5"/>
-        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2384,6 +2435,26 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -2394,12 +2465,6 @@
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i>
       <x v="4"/>
@@ -2417,10 +2482,16 @@
       <x v="9"/>
     </i>
     <i>
-      <x v="10"/>
+      <x v="11"/>
     </i>
     <i>
-      <x v="11"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i t="grand">
       <x/>
@@ -2445,6 +2516,12 @@
       <x/>
     </i>
   </colItems>
+  <pageFields count="4">
+    <pageField fld="10" hier="-1"/>
+    <pageField fld="7" hier="-1"/>
+    <pageField fld="8" hier="-1"/>
+    <pageField fld="9" hier="-1"/>
+  </pageFields>
   <dataFields count="2">
     <dataField name="NoSQL" fld="2" baseField="0" baseItem="0"/>
     <dataField name="Relational" fld="3" baseField="0" baseItem="0"/>
@@ -2716,23 +2793,26 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A1:E15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A6:E20" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
-      <items count="13">
+      <items count="16">
         <item x="0"/>
         <item x="1"/>
-        <item x="8"/>
-        <item x="9"/>
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
         <item x="2"/>
         <item x="3"/>
-        <item m="1" x="11"/>
+        <item m="1" x="14"/>
         <item x="6"/>
         <item x="10"/>
         <item x="4"/>
+        <item m="1" x="12"/>
+        <item x="7"/>
         <item x="5"/>
-        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2747,6 +2827,26 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0" defaultSubtotal="0">
+      <items count="1">
+        <item x="0"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -2757,12 +2857,6 @@
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i>
       <x v="4"/>
@@ -2780,10 +2874,16 @@
       <x v="9"/>
     </i>
     <i>
-      <x v="10"/>
+      <x v="11"/>
     </i>
     <i>
-      <x v="11"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i t="grand">
       <x/>
@@ -2808,6 +2908,12 @@
       <x/>
     </i>
   </colItems>
+  <pageFields count="4">
+    <pageField fld="10" hier="-1"/>
+    <pageField fld="7" hier="-1"/>
+    <pageField fld="8" hier="-1"/>
+    <pageField fld="9" hier="-1"/>
+  </pageFields>
   <dataFields count="2">
     <dataField name="NoSQL" fld="4" baseField="0" baseItem="0"/>
     <dataField name="Relational" fld="5" baseField="0" baseItem="0"/>
@@ -3046,9 +3152,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:G12" totalsRowShown="0">
-  <autoFilter ref="A1:G12"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K12" totalsRowShown="0">
+  <autoFilter ref="A1:K12"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="Bench type"/>
     <tableColumn id="2" name="Simple"/>
     <tableColumn id="3" name="Standard objects"/>
@@ -3056,6 +3162,10 @@
     <tableColumn id="5" name="Complex objects"/>
     <tableColumn id="6" name="Complex relations"/>
     <tableColumn id="7" name="Target"/>
+    <tableColumn id="8" name="Database"/>
+    <tableColumn id="9" name="Platform"/>
+    <tableColumn id="10" name="ORM"/>
+    <tableColumn id="11" name="API"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3348,11 +3458,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3363,11 +3471,13 @@
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3385,10 +3495,22 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3408,10 +3530,22 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3431,10 +3565,22 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3454,10 +3600,22 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3477,10 +3635,22 @@
         <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3500,145 +3670,229 @@
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="G8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="G9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
         <v>82</v>
       </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="I10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="F10" t="s">
+      <c r="C11" t="s">
         <v>57</v>
       </c>
-      <c r="G10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>61</v>
       </c>
-      <c r="E11" t="s">
+      <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="F11" t="s">
+      <c r="C12" t="s">
         <v>63</v>
       </c>
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>69</v>
       </c>
-      <c r="G12" t="s">
-        <v>72</v>
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3652,10 +3906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A8" sqref="A8:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,81 +3942,58 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3773,7 +4004,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -3784,7 +4015,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -3795,7 +4026,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -3806,7 +4037,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -3817,7 +4048,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -3828,12 +4059,67 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
       </c>
       <c r="C14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3845,10 +4131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,120 +4167,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>73</v>
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
+      <c r="A8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -4011,7 +4244,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -4028,7 +4261,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -4045,7 +4278,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -4062,7 +4295,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -4079,7 +4312,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -4096,7 +4329,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -4108,6 +4341,91 @@
         <v>0</v>
       </c>
       <c r="E15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4119,11 +4437,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4155,120 +4471,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>73</v>
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
+      <c r="A8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -4285,7 +4548,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -4302,7 +4565,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -4319,7 +4582,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -4336,7 +4599,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -4353,7 +4616,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -4370,7 +4633,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -4382,6 +4645,91 @@
         <v>0</v>
       </c>
       <c r="E15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>